<commit_message>
Logbook les update + vandaag
</commit_message>
<xml_diff>
--- a/Map2.xlsx
+++ b/Map2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gleb\Documents\UCLL\1.2\Dataquery\dbr01_g08\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levin\Documents\school - uclll\Semester 2\Querrying\repository\dbr01_g08\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B9491B-4DFA-43DB-BD99-AE62CF9091EB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>datum</t>
   </si>
@@ -42,12 +43,18 @@
   </si>
   <si>
     <t xml:space="preserve">Git aan gemaakt, toevoegen van twee tabellen </t>
+  </si>
+  <si>
+    <t>Create Drop Insert into</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Drop </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -359,11 +366,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,6 +406,45 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>43227</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>43234</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>43236</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>